<commit_message>
Now creating plotly graph from notebook
</commit_message>
<xml_diff>
--- a/data/interim/iva_kumulativ.xlsx
+++ b/data/interim/iva_kumulativ.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB22"/>
+  <dimension ref="A1:AC23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -507,6 +507,11 @@
           <t>2020-04-01</t>
         </is>
       </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>2020-04-02</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -591,6 +596,9 @@
       <c r="AB2" t="n">
         <v>1</v>
       </c>
+      <c r="AC2" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -679,6 +687,9 @@
       <c r="AB3" t="n">
         <v>12</v>
       </c>
+      <c r="AC3" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -767,6 +778,9 @@
       <c r="AB4" t="n">
         <v>12</v>
       </c>
+      <c r="AC4" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -854,6 +868,9 @@
       </c>
       <c r="AB5" t="n">
         <v>8</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="6">
@@ -915,6 +932,9 @@
       <c r="AB6" t="n">
         <v>1</v>
       </c>
+      <c r="AC6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -1003,6 +1023,9 @@
       <c r="AB7" t="n">
         <v>13</v>
       </c>
+      <c r="AC7" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -1091,6 +1114,9 @@
       <c r="AB8" t="n">
         <v>2</v>
       </c>
+      <c r="AC8" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -1177,6 +1203,9 @@
         <v>0</v>
       </c>
       <c r="AB9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1239,6 +1268,9 @@
       <c r="AB10" t="n">
         <v>18</v>
       </c>
+      <c r="AC10" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -1327,6 +1359,9 @@
       <c r="AB11" t="n">
         <v>26</v>
       </c>
+      <c r="AC11" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -1415,6 +1450,9 @@
       <c r="AB12" t="n">
         <v>224</v>
       </c>
+      <c r="AC12" t="n">
+        <v>247</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -1502,6 +1540,9 @@
       </c>
       <c r="AB13" t="n">
         <v>44</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>46</v>
       </c>
     </row>
     <row r="14">
@@ -1577,6 +1618,9 @@
       <c r="AB14" t="n">
         <v>17</v>
       </c>
+      <c r="AC14" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -1665,6 +1709,9 @@
       <c r="AB15" t="n">
         <v>4</v>
       </c>
+      <c r="AC15" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -1753,6 +1800,9 @@
       <c r="AB16" t="n">
         <v>6</v>
       </c>
+      <c r="AC16" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -1841,6 +1891,9 @@
       <c r="AB17" t="n">
         <v>5</v>
       </c>
+      <c r="AC17" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -1929,6 +1982,9 @@
       <c r="AB18" t="n">
         <v>13</v>
       </c>
+      <c r="AC18" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -2017,6 +2073,9 @@
       <c r="AB19" t="n">
         <v>14</v>
       </c>
+      <c r="AC19" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -2105,6 +2164,9 @@
       <c r="AB20" t="n">
         <v>29</v>
       </c>
+      <c r="AC20" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -2193,6 +2255,9 @@
       <c r="AB21" t="n">
         <v>77</v>
       </c>
+      <c r="AC21" t="n">
+        <v>79</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -2280,6 +2345,46 @@
       </c>
       <c r="AB22" t="n">
         <v>526</v>
+      </c>
+      <c r="AC22" t="n">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>Region Gotland</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr"/>
+      <c r="R23" t="inlineStr"/>
+      <c r="S23" t="inlineStr"/>
+      <c r="T23" t="inlineStr"/>
+      <c r="U23" t="inlineStr"/>
+      <c r="V23" t="inlineStr"/>
+      <c r="W23" t="inlineStr"/>
+      <c r="X23" t="inlineStr"/>
+      <c r="Y23" t="inlineStr"/>
+      <c r="Z23" t="inlineStr"/>
+      <c r="AA23" t="inlineStr"/>
+      <c r="AB23" t="inlineStr"/>
+      <c r="AC23" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Addera utskrivningar samt uppdatering vid ny iva-data
</commit_message>
<xml_diff>
--- a/data/interim/iva_kumulativ.xlsx
+++ b/data/interim/iva_kumulativ.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC23"/>
+  <dimension ref="A1:AD23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,6 +512,11 @@
           <t>2020-04-02</t>
         </is>
       </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>2020-04-03</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -599,6 +604,9 @@
       <c r="AC2" t="n">
         <v>2</v>
       </c>
+      <c r="AD2" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -664,31 +672,34 @@
         <v>5</v>
       </c>
       <c r="U3" t="n">
+        <v>7</v>
+      </c>
+      <c r="V3" t="n">
         <v>8</v>
       </c>
-      <c r="V3" t="n">
+      <c r="W3" t="n">
+        <v>8</v>
+      </c>
+      <c r="X3" t="n">
+        <v>8</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>8</v>
+      </c>
+      <c r="Z3" t="n">
         <v>9</v>
       </c>
-      <c r="W3" t="n">
+      <c r="AA3" t="n">
         <v>9</v>
       </c>
-      <c r="X3" t="n">
+      <c r="AB3" t="n">
         <v>10</v>
       </c>
-      <c r="Y3" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z3" t="n">
+      <c r="AC3" t="n">
         <v>11</v>
       </c>
-      <c r="AA3" t="n">
+      <c r="AD3" t="n">
         <v>11</v>
-      </c>
-      <c r="AB3" t="n">
-        <v>12</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>13</v>
       </c>
     </row>
     <row r="4">
@@ -752,33 +763,36 @@
         <v>2</v>
       </c>
       <c r="T4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="X4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Y4" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Z4" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AA4" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AB4" t="n">
+        <v>11</v>
+      </c>
+      <c r="AC4" t="n">
         <v>12</v>
       </c>
-      <c r="AC4" t="n">
+      <c r="AD4" t="n">
         <v>14</v>
       </c>
     </row>
@@ -870,6 +884,9 @@
         <v>8</v>
       </c>
       <c r="AC5" t="n">
+        <v>10</v>
+      </c>
+      <c r="AD5" t="n">
         <v>10</v>
       </c>
     </row>
@@ -935,6 +952,9 @@
       <c r="AC6" t="n">
         <v>1</v>
       </c>
+      <c r="AD6" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -1026,6 +1046,9 @@
       <c r="AC7" t="n">
         <v>15</v>
       </c>
+      <c r="AD7" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -1117,6 +1140,9 @@
       <c r="AC8" t="n">
         <v>4</v>
       </c>
+      <c r="AD8" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -1206,6 +1232,9 @@
         <v>0</v>
       </c>
       <c r="AC9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1233,43 +1262,46 @@
         <v>1</v>
       </c>
       <c r="Q10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R10" t="n">
+        <v>3</v>
+      </c>
+      <c r="S10" t="n">
+        <v>3</v>
+      </c>
+      <c r="T10" t="n">
         <v>5</v>
       </c>
-      <c r="S10" t="n">
-        <v>6</v>
-      </c>
-      <c r="T10" t="n">
+      <c r="U10" t="n">
+        <v>5</v>
+      </c>
+      <c r="V10" t="n">
+        <v>7</v>
+      </c>
+      <c r="W10" t="n">
+        <v>7</v>
+      </c>
+      <c r="X10" t="n">
+        <v>7</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>8</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>9</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>9</v>
+      </c>
+      <c r="AC10" t="n">
         <v>10</v>
       </c>
-      <c r="U10" t="n">
+      <c r="AD10" t="n">
         <v>10</v>
-      </c>
-      <c r="V10" t="n">
-        <v>12</v>
-      </c>
-      <c r="W10" t="n">
-        <v>14</v>
-      </c>
-      <c r="X10" t="n">
-        <v>14</v>
-      </c>
-      <c r="Y10" t="n">
-        <v>15</v>
-      </c>
-      <c r="Z10" t="n">
-        <v>16</v>
-      </c>
-      <c r="AA10" t="n">
-        <v>18</v>
-      </c>
-      <c r="AB10" t="n">
-        <v>18</v>
-      </c>
-      <c r="AC10" t="n">
-        <v>20</v>
       </c>
     </row>
     <row r="11">
@@ -1321,46 +1353,49 @@
         <v>6</v>
       </c>
       <c r="P11" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>8</v>
+      </c>
+      <c r="R11" t="n">
+        <v>8</v>
+      </c>
+      <c r="S11" t="n">
         <v>9</v>
       </c>
-      <c r="Q11" t="n">
+      <c r="T11" t="n">
         <v>9</v>
       </c>
-      <c r="R11" t="n">
+      <c r="U11" t="n">
         <v>9</v>
       </c>
-      <c r="S11" t="n">
-        <v>11</v>
-      </c>
-      <c r="T11" t="n">
-        <v>11</v>
-      </c>
-      <c r="U11" t="n">
-        <v>11</v>
-      </c>
       <c r="V11" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="W11" t="n">
+        <v>13</v>
+      </c>
+      <c r="X11" t="n">
+        <v>14</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>14</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>14</v>
+      </c>
+      <c r="AA11" t="n">
         <v>16</v>
       </c>
-      <c r="X11" t="n">
+      <c r="AB11" t="n">
+        <v>18</v>
+      </c>
+      <c r="AC11" t="n">
         <v>19</v>
       </c>
-      <c r="Y11" t="n">
+      <c r="AD11" t="n">
         <v>19</v>
-      </c>
-      <c r="Z11" t="n">
-        <v>19</v>
-      </c>
-      <c r="AA11" t="n">
-        <v>23</v>
-      </c>
-      <c r="AB11" t="n">
-        <v>26</v>
-      </c>
-      <c r="AC11" t="n">
-        <v>29</v>
       </c>
     </row>
     <row r="12">
@@ -1370,88 +1405,91 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I12" t="n">
+        <v>4</v>
+      </c>
+      <c r="J12" t="n">
         <v>6</v>
       </c>
-      <c r="J12" t="n">
-        <v>9</v>
-      </c>
       <c r="K12" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="L12" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="M12" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="N12" t="n">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="O12" t="n">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="P12" t="n">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="Q12" t="n">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="R12" t="n">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="S12" t="n">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="T12" t="n">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="U12" t="n">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="V12" t="n">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="W12" t="n">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="X12" t="n">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="Y12" t="n">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="Z12" t="n">
-        <v>192</v>
+        <v>163</v>
       </c>
       <c r="AA12" t="n">
-        <v>208</v>
+        <v>176</v>
       </c>
       <c r="AB12" t="n">
-        <v>224</v>
+        <v>191</v>
       </c>
       <c r="AC12" t="n">
-        <v>247</v>
+        <v>211</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>229</v>
       </c>
     </row>
     <row r="13">
@@ -1503,46 +1541,49 @@
         <v>2</v>
       </c>
       <c r="P13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q13" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="R13" t="n">
+        <v>10</v>
+      </c>
+      <c r="S13" t="n">
         <v>12</v>
       </c>
-      <c r="S13" t="n">
-        <v>14</v>
-      </c>
       <c r="T13" t="n">
+        <v>18</v>
+      </c>
+      <c r="U13" t="n">
         <v>20</v>
       </c>
-      <c r="U13" t="n">
+      <c r="V13" t="n">
         <v>22</v>
       </c>
-      <c r="V13" t="n">
+      <c r="W13" t="n">
         <v>24</v>
       </c>
-      <c r="W13" t="n">
-        <v>26</v>
-      </c>
       <c r="X13" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Y13" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="Z13" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA13" t="n">
         <v>37</v>
       </c>
-      <c r="AA13" t="n">
-        <v>41</v>
-      </c>
       <c r="AB13" t="n">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="AC13" t="n">
-        <v>46</v>
+        <v>42</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="14">
@@ -1595,31 +1636,34 @@
         <v>6</v>
       </c>
       <c r="U14" t="n">
+        <v>8</v>
+      </c>
+      <c r="V14" t="n">
         <v>9</v>
       </c>
-      <c r="V14" t="n">
-        <v>10</v>
-      </c>
       <c r="W14" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="X14" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Y14" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Z14" t="n">
+        <v>14</v>
+      </c>
+      <c r="AA14" t="n">
         <v>15</v>
       </c>
-      <c r="AA14" t="n">
+      <c r="AB14" t="n">
         <v>16</v>
       </c>
-      <c r="AB14" t="n">
-        <v>17</v>
-      </c>
       <c r="AC14" t="n">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="15">
@@ -1712,6 +1756,9 @@
       <c r="AC15" t="n">
         <v>4</v>
       </c>
+      <c r="AD15" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -1803,6 +1850,9 @@
       <c r="AC16" t="n">
         <v>8</v>
       </c>
+      <c r="AD16" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -1865,34 +1915,37 @@
         <v>1</v>
       </c>
       <c r="T17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="X17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Y17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Z17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AA17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB17" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC17" t="n">
         <v>5</v>
       </c>
-      <c r="AC17" t="n">
-        <v>6</v>
+      <c r="AD17" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="18">
@@ -1971,19 +2024,22 @@
         <v>9</v>
       </c>
       <c r="Y18" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Z18" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AA18" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AB18" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AC18" t="n">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="AD18" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="19">
@@ -2050,31 +2106,34 @@
         <v>4</v>
       </c>
       <c r="U19" t="n">
+        <v>6</v>
+      </c>
+      <c r="V19" t="n">
         <v>7</v>
       </c>
-      <c r="V19" t="n">
-        <v>8</v>
-      </c>
       <c r="W19" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="X19" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Y19" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Z19" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AA19" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AB19" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AC19" t="n">
-        <v>16</v>
+        <v>12</v>
+      </c>
+      <c r="AD19" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="20">
@@ -2153,19 +2212,22 @@
         <v>25</v>
       </c>
       <c r="Y20" t="n">
+        <v>27</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>27</v>
+      </c>
+      <c r="AA20" t="n">
         <v>28</v>
       </c>
-      <c r="Z20" t="n">
+      <c r="AB20" t="n">
         <v>28</v>
       </c>
-      <c r="AA20" t="n">
-        <v>29</v>
-      </c>
-      <c r="AB20" t="n">
-        <v>29</v>
-      </c>
       <c r="AC20" t="n">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="AD20" t="n">
+        <v>36</v>
       </c>
     </row>
     <row r="21">
@@ -2214,49 +2276,52 @@
         <v>6</v>
       </c>
       <c r="O21" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P21" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>12</v>
+      </c>
+      <c r="R21" t="n">
         <v>14</v>
       </c>
-      <c r="Q21" t="n">
+      <c r="S21" t="n">
         <v>18</v>
       </c>
-      <c r="R21" t="n">
-        <v>21</v>
-      </c>
-      <c r="S21" t="n">
-        <v>26</v>
-      </c>
       <c r="T21" t="n">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="U21" t="n">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="V21" t="n">
+        <v>25</v>
+      </c>
+      <c r="W21" t="n">
+        <v>27</v>
+      </c>
+      <c r="X21" t="n">
+        <v>31</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>37</v>
+      </c>
+      <c r="Z21" t="n">
         <v>40</v>
       </c>
-      <c r="W21" t="n">
+      <c r="AA21" t="n">
         <v>44</v>
       </c>
-      <c r="X21" t="n">
+      <c r="AB21" t="n">
         <v>49</v>
       </c>
-      <c r="Y21" t="n">
-        <v>60</v>
-      </c>
-      <c r="Z21" t="n">
-        <v>65</v>
-      </c>
-      <c r="AA21" t="n">
-        <v>70</v>
-      </c>
-      <c r="AB21" t="n">
-        <v>77</v>
-      </c>
       <c r="AC21" t="n">
-        <v>79</v>
+        <v>50</v>
+      </c>
+      <c r="AD21" t="n">
+        <v>54</v>
       </c>
     </row>
     <row r="22">
@@ -2266,88 +2331,91 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D22" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E22" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22" t="n">
+        <v>6</v>
+      </c>
+      <c r="G22" t="n">
+        <v>6</v>
+      </c>
+      <c r="H22" t="n">
         <v>7</v>
       </c>
-      <c r="G22" t="n">
-        <v>7</v>
-      </c>
-      <c r="H22" t="n">
-        <v>8</v>
-      </c>
       <c r="I22" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J22" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="K22" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="L22" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="M22" t="n">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="N22" t="n">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="O22" t="n">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="P22" t="n">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="Q22" t="n">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="R22" t="n">
-        <v>130</v>
+        <v>104</v>
       </c>
       <c r="S22" t="n">
-        <v>175</v>
+        <v>142</v>
       </c>
       <c r="T22" t="n">
-        <v>218</v>
+        <v>176</v>
       </c>
       <c r="U22" t="n">
-        <v>259</v>
+        <v>206</v>
       </c>
       <c r="V22" t="n">
+        <v>245</v>
+      </c>
+      <c r="W22" t="n">
+        <v>272</v>
+      </c>
+      <c r="X22" t="n">
         <v>300</v>
       </c>
-      <c r="W22" t="n">
-        <v>332</v>
-      </c>
-      <c r="X22" t="n">
-        <v>367</v>
-      </c>
       <c r="Y22" t="n">
-        <v>413</v>
+        <v>336</v>
       </c>
       <c r="Z22" t="n">
-        <v>449</v>
+        <v>364</v>
       </c>
       <c r="AA22" t="n">
-        <v>483</v>
+        <v>391</v>
       </c>
       <c r="AB22" t="n">
-        <v>526</v>
+        <v>427</v>
       </c>
       <c r="AC22" t="n">
-        <v>584</v>
+        <v>477</v>
+      </c>
+      <c r="AD22" t="n">
+        <v>514</v>
       </c>
     </row>
     <row r="23">
@@ -2386,6 +2454,9 @@
       <c r="AC23" t="n">
         <v>1</v>
       </c>
+      <c r="AD23" t="n">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>